<commit_message>
fix years of experience (in progress)
</commit_message>
<xml_diff>
--- a/data/Professional Personnel Individual Staff Report Notes and Data Elements.xlsx
+++ b/data/Professional Personnel Individual Staff Report Notes and Data Elements.xlsx
@@ -752,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0661E917-906F-400D-B5A3-9EA67EC482DB}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1192,6 +1192,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010063A4E9D8B9AE294BB8664582FC3229C4" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ab5e3be8eaf3cd0fb5535aa68510e8f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="daabebb8d57a36d92a4894986269ef22" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1323,25 +1341,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{215A6A75-0FBB-4F1F-A3EA-2976B643DE37}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D9F211E-74D6-4B6B-8B2F-BD3C1A44CEC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5AA5F4E-387C-4DF8-9315-D30F60A4E065}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1357,22 +1375,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D9F211E-74D6-4B6B-8B2F-BD3C1A44CEC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{215A6A75-0FBB-4F1F-A3EA-2976B643DE37}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>